<commit_message>
New guide to macro
</commit_message>
<xml_diff>
--- a/Info/site checklist.xlsx
+++ b/Info/site checklist.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xsunde/Dropbox/Jupyter/stathelp/Info/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797BAF8F-7E8D-8D41-9B7D-D019E4F44C7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26519"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7520" yWindow="3120" windowWidth="25640" windowHeight="17060" xr2:uid="{4564286C-4F44-964C-BD91-BFFA18ED1E63}"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -230,7 +227,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -274,7 +271,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Procent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -332,7 +329,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -384,7 +381,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -578,21 +575,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1B1993-1316-8847-B352-6843485D5D83}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
@@ -603,7 +600,7 @@
     <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="B1" t="s">
         <v>61</v>
       </c>
@@ -612,25 +609,25 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="B2" t="s">
         <v>47</v>
       </c>
       <c r="C2">
         <f>SUM(C10:C197)</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="B3" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="1">
         <f>C2/C1</f>
-        <v>0.52272727272727271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.54545454545454541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="B4" t="s">
         <v>48</v>
       </c>
@@ -639,22 +636,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="B5" t="s">
         <v>49</v>
       </c>
       <c r="C5" s="1">
         <f>C4/C2</f>
-        <v>0.60869565217391308</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="D6">
         <f>G2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -677,7 +674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -703,7 +700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -717,12 +714,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -748,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -771,7 +768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -794,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -817,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -831,7 +828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -854,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -877,17 +874,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="B21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="B22" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -895,32 +892,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="B25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="B26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="B27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="B28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="B29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -928,17 +925,17 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="B32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="B33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -964,7 +961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="B36" t="s">
         <v>23</v>
       </c>
@@ -978,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="B37" t="s">
         <v>24</v>
       </c>
@@ -1001,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="B38" t="s">
         <v>25</v>
       </c>
@@ -1024,7 +1021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="B39" t="s">
         <v>26</v>
       </c>
@@ -1047,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="B40" t="s">
         <v>27</v>
       </c>
@@ -1061,17 +1058,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="B41" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="B42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -1097,12 +1103,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="B45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="B46" t="s">
         <v>34</v>
       </c>
@@ -1116,7 +1122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="B47" t="s">
         <v>35</v>
       </c>
@@ -1139,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="B48" t="s">
         <v>36</v>
       </c>
@@ -1153,22 +1159,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="B49" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="B50" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="B51" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>41</v>
       </c>
@@ -1185,7 +1191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="B54" t="s">
         <v>43</v>
       </c>
@@ -1199,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9">
       <c r="B55" t="s">
         <v>44</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9">
       <c r="B56" t="s">
         <v>45</v>
       </c>
@@ -1236,12 +1242,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9">
       <c r="B57" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9">
       <c r="A61" t="s">
         <v>29</v>
       </c>
@@ -1249,17 +1255,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9">
       <c r="B62" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9">
       <c r="B63" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Translated merge guide to EN
</commit_message>
<xml_diff>
--- a/Info/site checklist.xlsx
+++ b/Info/site checklist.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26519"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xsunde/Dropbox/Jupyter/stathelp/Info/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E153FBB0-F02C-2142-9428-055961B35FF8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280"/>
+    <workbookView xWindow="7520" yWindow="3120" windowWidth="25640" windowHeight="17060" xr2:uid="{4564286C-4F44-964C-BD91-BFFA18ED1E63}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -227,8 +230,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,6 +240,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -265,13 +276,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Procent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -329,7 +341,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -381,7 +393,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -575,24 +587,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB1B1993-1316-8847-B352-6843485D5D83}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
@@ -600,7 +612,7 @@
     <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>61</v>
       </c>
@@ -609,25 +621,25 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>47</v>
       </c>
       <c r="C2">
         <f>SUM(C10:C197)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="1">
         <f>C2/C1</f>
-        <v>0.54545454545454541</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0.52272727272727271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>48</v>
       </c>
@@ -636,22 +648,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>49</v>
       </c>
       <c r="C5" s="1">
         <f>C4/C2</f>
-        <v>0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0.60869565217391308</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D6">
         <f>G2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -674,7 +686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -700,7 +712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -714,12 +726,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -745,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -768,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -791,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -814,7 +826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -828,7 +840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -851,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -874,17 +886,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -892,32 +904,32 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>56</v>
       </c>
@@ -925,17 +937,17 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -961,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>23</v>
       </c>
@@ -975,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>24</v>
       </c>
@@ -998,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>25</v>
       </c>
@@ -1021,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>26</v>
       </c>
@@ -1044,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>27</v>
       </c>
@@ -1054,30 +1066,18 @@
       <c r="D40">
         <v>1</v>
       </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>64</v>
       </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -1103,12 +1103,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>34</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>35</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>36</v>
       </c>
@@ -1159,22 +1159,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>41</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>43</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>44</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>45</v>
       </c>
@@ -1242,12 +1242,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>29</v>
       </c>
@@ -1255,22 +1255,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>